<commit_message>
Updated with prediction for final
</commit_message>
<xml_diff>
--- a/data/Final4Data.xlsx
+++ b/data/Final4Data.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec Otterson\AlecDocs\BYUI\AI Society\SCAI\cs450_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Isaac School\CS 450\Project\cs450_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E35C844-8D88-42DA-9683-784181C4ECF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6C3A13-5D88-440A-A22A-558FE5F8C980}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEF1B953-57F1-4561-9CAE-4B9F564F8BBF}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{AEF1B953-57F1-4561-9CAE-4B9F564F8BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -96,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,8 +126,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{364483B6-6658-492D-A440-A1A14B758961}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -445,12 +467,12 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,12 +534,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2">
         <v>1403</v>
       </c>
       <c r="C2">
         <v>1277</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <f>75-68</f>
@@ -582,12 +610,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
       <c r="B3">
         <v>1120</v>
       </c>
       <c r="C3">
         <v>1438</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
         <f>77-80</f>

</xml_diff>